<commit_message>
module : pabi_procurement_report PO: เพิ่มรายงาน Book Stock Balance ในเมนู Sales Issues : https://mobileapp.nstda.or.th/redmine/issues/4031
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_book_stock_balance.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_book_stock_balance.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>ศูนย์</t>
   </si>
@@ -450,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="A8" sqref="A8:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -469,7 +469,7 @@
     <col min="10" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
@@ -479,7 +479,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -489,7 +489,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:10" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -499,7 +499,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:10" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="8" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -509,14 +509,14 @@
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -546,6 +546,9 @@
       </c>
       <c r="J7" s="5" t="s">
         <v>9</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>